<commit_message>
+Converted numbers to int(floor and ceil)
</commit_message>
<xml_diff>
--- a/Data/Input/input_UIDemo.xlsx
+++ b/Data/Input/input_UIDemo.xlsx
@@ -3,13 +3,14 @@
 <x:workbook xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D73DA2-6E22-45E6-BE69-AA7A194AB955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0123BBA0-9AF8-4DDC-B709-CA9F29842804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Sheet2" sheetId="8" r:id="rId8"/>
+    <x:sheet name="Sheet2" sheetId="8" r:id="rId2"/>
+    <x:sheet name="Sheet3" sheetId="9" r:id="rId9"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191028"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <x:si>
     <x:t>CashIn</x:t>
   </x:si>
@@ -63,157 +64,292 @@
     <x:t>C146</x:t>
   </x:si>
   <x:si>
-    <x:t>403494</x:t>
+    <x:t>715431</x:t>
   </x:si>
   <x:si>
     <x:t>Success</x:t>
   </x:si>
   <x:si>
-    <x:t>403495</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403496</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403497</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403498</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403499</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403500</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403501</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403502</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403503</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403504</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403505</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403506</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403507</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403508</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403509</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403510</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403511</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403512</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403513</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403514</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403515</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403516</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403517</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403518</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403519</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403520</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403521</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403522</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403523</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403524</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403525</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403526</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403527</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403528</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403529</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403530</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403531</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403532</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403533</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403534</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403535</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403536</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403537</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403538</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403539</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403540</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403541</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403542</x:t>
-  </x:si>
-  <x:si>
-    <x:t>403543</x:t>
+    <x:t>No Exception</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715432</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715433</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715434</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715435</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Failed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Business Exception</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715436</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715437</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715438</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715439</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715440</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715441</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715442</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715443</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715444</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715445</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715446</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715447</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715448</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715449</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715450</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715451</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715452</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715453</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715454</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715455</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715456</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715457</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715458</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715459</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715460</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715461</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715462</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715463</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715464</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715465</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715466</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715467</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715468</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715469</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715470</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715471</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715472</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715473</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715474</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715475</x:t>
+  </x:si>
+  <x:si>
+    <x:t>715476</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851095</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851096</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851097</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851098</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851099</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851101</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851102</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851103</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851104</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851105</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851106</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851107</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851108</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851109</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851110</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851111</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851113</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851114</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851115</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851116</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851117</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851118</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851119</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851120</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851121</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851122</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851124</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851125</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851126</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851127</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851128</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851129</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851130</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851131</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851132</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851133</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851134</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851135</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851136</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851137</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851138</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851139</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851140</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -591,7 +727,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:F51"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="H9" sqref="H9"/>
     </x:sheetView>
   </x:sheetViews>
@@ -1177,6 +1313,1034 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F51"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="n">
+        <x:v>911.07</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="n">
+        <x:v>231.36</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="n">
+        <x:v>897.56</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
+        <x:v>528.85</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="0" t="n">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>997.34</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="0" t="n">
+        <x:v>484.04</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
+        <x:v>388.6</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="0" t="n">
+        <x:v>329.5</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>669.55</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="0" t="n">
+        <x:v>374.31</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="n">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="0" t="n">
+        <x:v>86.43</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="n">
+        <x:v>682.58</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="0" t="n">
+        <x:v>599.98</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="n">
+        <x:v>872.16</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="0" t="n">
+        <x:v>446.53</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="n">
+        <x:v>778.83</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="n">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="0" t="n">
+        <x:v>662.42</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="n">
+        <x:v>184.2</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="0" t="n">
+        <x:v>560.55</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="n">
+        <x:v>203.93</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="n">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="0" t="n">
+        <x:v>115.34</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="n">
+        <x:v>552.88</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="n">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="0" t="n">
+        <x:v>262.48</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="n">
+        <x:v>830.91</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="0" t="n">
+        <x:v>840.24</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="n">
+        <x:v>685.89</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="0" t="n">
+        <x:v>737.16</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="n">
+        <x:v>524.21</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="n">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="n">
+        <x:v>402.85</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="n">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="0" t="n">
+        <x:v>147.54</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="n">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="0" t="n">
+        <x:v>980.09</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="n">
+        <x:v>99.64</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="0" t="n">
+        <x:v>408.62</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="n">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A21" s="0" t="n">
+        <x:v>349.37</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="n">
+        <x:v>290.87</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="n">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A22" s="0" t="n">
+        <x:v>794.12</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="n">
+        <x:v>432.29</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="n">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A23" s="0" t="n">
+        <x:v>89.77</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="n">
+        <x:v>167.9</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="n">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A24" s="0" t="n">
+        <x:v>40.43</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="n">
+        <x:v>3.03</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="n">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A25" s="0" t="n">
+        <x:v>40.33</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="n">
+        <x:v>480.28</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="n">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A26" s="0" t="n">
+        <x:v>1105.16</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="n">
+        <x:v>248.6</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="n">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A27" s="0" t="n">
+        <x:v>966.68</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="n">
+        <x:v>192.68</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="n">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A28" s="0" t="n">
+        <x:v>697.58</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="n">
+        <x:v>165.16</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="n">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A29" s="0" t="n">
+        <x:v>304.37</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="n">
+        <x:v>426.8</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A30" s="0" t="n">
+        <x:v>106.36</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="n">
+        <x:v>506.71</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A31" s="0" t="n">
+        <x:v>878.65</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="n">
+        <x:v>74.26</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="n">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A32" s="0" t="n">
+        <x:v>612.35</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="n">
+        <x:v>974.04</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="n">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A33" s="0" t="n">
+        <x:v>262.65</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="n">
+        <x:v>305.12</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="n">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A34" s="0" t="n">
+        <x:v>280.29</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="n">
+        <x:v>83.1</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="n">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A35" s="0" t="n">
+        <x:v>434.59</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="n">
+        <x:v>49.06</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="n">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A36" s="0" t="n">
+        <x:v>398.31</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="n">
+        <x:v>526.61</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="n">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A37" s="0" t="n">
+        <x:v>1028.43</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="n">
+        <x:v>55.02</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="n">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A38" s="0" t="n">
+        <x:v>1162.4</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="n">
+        <x:v>926.47</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A39" s="0" t="n">
+        <x:v>395.63</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="n">
+        <x:v>794.99</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A40" s="0" t="n">
+        <x:v>147.79</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="n">
+        <x:v>546.57</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="n">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A41" s="0" t="n">
+        <x:v>151.48</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="n">
+        <x:v>95.84</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A42" s="0" t="n">
+        <x:v>618.7</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="n">
+        <x:v>136.19</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="n">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A43" s="0" t="n">
+        <x:v>406.6</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="n">
+        <x:v>640.78</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A44" s="0" t="n">
+        <x:v>906.25</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="n">
+        <x:v>83.67</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="n">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A45" s="0" t="n">
+        <x:v>981.34</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="n">
+        <x:v>194.22</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A46" s="0" t="n">
+        <x:v>31.34</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="n">
+        <x:v>782.26</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="n">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A47" s="0" t="n">
+        <x:v>646.75</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="n">
+        <x:v>476.8</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A48" s="0" t="n">
+        <x:v>815.39</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="n">
+        <x:v>418.73</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="n">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A49" s="0" t="n">
+        <x:v>279.61</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="n">
+        <x:v>449.09</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="n">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A50" s="0" t="n">
+        <x:v>1010.27</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="n">
+        <x:v>695.52</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="n">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F50" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A51" s="0" t="n">
+        <x:v>821.17</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="n">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="n">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1218,13 +2382,13 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
@@ -1238,13 +2402,13 @@
         <x:v>180</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6">
@@ -1258,13 +2422,13 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
@@ -1278,13 +2442,13 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
@@ -1298,13 +2462,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
@@ -1317,14 +2481,11 @@
       <x:c r="C7" s="0" t="n">
         <x:v>112</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
@@ -1338,13 +2499,13 @@
         <x:v>104</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
@@ -1358,13 +2519,13 @@
         <x:v>155</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
@@ -1378,13 +2539,13 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6">
@@ -1398,13 +2559,13 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
@@ -1418,13 +2579,13 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:6">
@@ -1438,13 +2599,13 @@
         <x:v>164</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:6">
@@ -1458,13 +2619,13 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6">
@@ -1478,13 +2639,13 @@
         <x:v>70</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:6">
@@ -1498,13 +2659,13 @@
         <x:v>154</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
@@ -1517,14 +2678,11 @@
       <x:c r="C17" s="0" t="n">
         <x:v>82</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:6">
@@ -1538,13 +2696,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:6">
@@ -1558,13 +2716,13 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:6">
@@ -1577,14 +2735,11 @@
       <x:c r="C20" s="0" t="n">
         <x:v>126</x:v>
       </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:6">
@@ -1598,13 +2753,13 @@
         <x:v>124</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:6">
@@ -1618,13 +2773,13 @@
         <x:v>126</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:6">
@@ -1638,13 +2793,13 @@
         <x:v>186</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
@@ -1658,13 +2813,13 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:6">
@@ -1678,13 +2833,13 @@
         <x:v>132</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:6">
@@ -1698,13 +2853,13 @@
         <x:v>165</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:6">
@@ -1718,13 +2873,13 @@
         <x:v>175</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:6">
@@ -1738,13 +2893,13 @@
         <x:v>165</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:6">
@@ -1758,13 +2913,13 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:6">
@@ -1777,14 +2932,11 @@
       <x:c r="C30" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:6">
@@ -1798,13 +2950,13 @@
         <x:v>71</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:6">
@@ -1818,13 +2970,13 @@
         <x:v>168</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:6">
@@ -1838,13 +2990,13 @@
         <x:v>183</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="E33" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F33" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:6">
@@ -1858,13 +3010,13 @@
         <x:v>83</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E34" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F34" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:6">
@@ -1878,13 +3030,13 @@
         <x:v>156</x:v>
       </x:c>
       <x:c r="D35" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F35" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:6">
@@ -1898,13 +3050,13 @@
         <x:v>116</x:v>
       </x:c>
       <x:c r="D36" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="E36" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F36" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:6">
@@ -1918,13 +3070,13 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="E37" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:6">
@@ -1938,13 +3090,13 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="E38" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F38" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:6">
@@ -1958,13 +3110,13 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="D39" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E39" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F39" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:6">
@@ -1978,13 +3130,13 @@
         <x:v>161</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="E40" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:6">
@@ -1998,13 +3150,13 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="D41" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="E41" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F41" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:6">
@@ -2018,13 +3170,13 @@
         <x:v>85</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E42" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F42" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:6">
@@ -2038,13 +3190,13 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="E43" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:6">
@@ -2058,13 +3210,13 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="D44" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="E44" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F44" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:6">
@@ -2078,13 +3230,13 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="D45" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="E45" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F45" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:6">
@@ -2098,13 +3250,13 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="D46" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="E46" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F46" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:6">
@@ -2118,13 +3270,13 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D47" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E47" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:6">
@@ -2138,13 +3290,13 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="D48" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E48" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F48" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:6">
@@ -2158,13 +3310,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="D49" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="E49" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F49" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:6">
@@ -2178,13 +3330,13 @@
         <x:v>115</x:v>
       </x:c>
       <x:c r="D50" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="E50" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F50" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:6">
@@ -2198,13 +3350,13 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="D51" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E51" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="F51" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>